<commit_message>
Figuring out RNA sequencing strategy
</commit_message>
<xml_diff>
--- a/picking_samples_final.xlsx
+++ b/picking_samples_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurabogar/Documents/One Plant One Fungus/Hebeloma/Hebeloma_drydown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7A6981-C3B3-714A-A99C-ECE0919F9DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29930CB-496A-5149-AD1B-488D71A1C830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="27640" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="500" windowWidth="27640" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_for_picking_samples" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="300">
   <si>
     <t>harvest_day</t>
   </si>
@@ -811,6 +811,132 @@
   </si>
   <si>
     <t>DNA:RNA ratio</t>
+  </si>
+  <si>
+    <t>Extraction tube</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>1G</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>2F</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>3E</t>
+  </si>
+  <si>
+    <t>3F</t>
+  </si>
+  <si>
+    <t>3G</t>
+  </si>
+  <si>
+    <t>3H</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>4C</t>
+  </si>
+  <si>
+    <t>4D</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>4H</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Tube letter</t>
+  </si>
+  <si>
+    <t>Target 6/2?</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1491,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1412,6 +1538,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1457,7 +1586,57 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1727,17 +1906,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C633DB3-6EE1-BE4B-9003-30AD2C5AADEB}" name="Table2" displayName="Table2" ref="A1:H33" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H33" xr:uid="{8C633DB3-6EE1-BE4B-9003-30AD2C5AADEB}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3C07F592-4BB5-384C-A9F5-414B5E307493}" name="Extraction batch" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{2D2FABD1-B976-E04D-B06C-C53294602B17}" name="harvest_day" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{78FA34BA-1883-1647-8C42-33DD93C4ECA1}" name="seedling" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{AC2049CC-0B8E-4E47-BBCD-4A7A746FADB9}" name="water" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{BC3723B5-324B-6147-B568-90FB568E69B4}" name="n" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{4A60710D-FED5-6842-8D63-A7390C5B0A5B}" name="colonized" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{BB4EFFED-F5E1-4944-B8BC-227F1B176BDF}" name="corrected_phi" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{95228BDC-BE3E-F340-A3CA-A07507AC98CD}" name="Group for analysis" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C633DB3-6EE1-BE4B-9003-30AD2C5AADEB}" name="Table2" displayName="Table2" ref="A1:J33" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J33" xr:uid="{8C633DB3-6EE1-BE4B-9003-30AD2C5AADEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J33">
+    <sortCondition ref="I1:I33"/>
+  </sortState>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{3C07F592-4BB5-384C-A9F5-414B5E307493}" name="Extraction batch" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{2D2FABD1-B976-E04D-B06C-C53294602B17}" name="harvest_day" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{78FA34BA-1883-1647-8C42-33DD93C4ECA1}" name="seedling" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{AC2049CC-0B8E-4E47-BBCD-4A7A746FADB9}" name="water" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{BC3723B5-324B-6147-B568-90FB568E69B4}" name="n" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A60710D-FED5-6842-8D63-A7390C5B0A5B}" name="colonized" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{BB4EFFED-F5E1-4944-B8BC-227F1B176BDF}" name="corrected_phi" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{95228BDC-BE3E-F340-A3CA-A07507AC98CD}" name="Group for analysis" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{3CEA81C4-964C-9349-A08E-198EB3BEC1FB}" name="Extraction tube" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{8BD5BC28-12AF-5845-9074-8738ABAA8607}" name="Tube letter" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2040,11 +2224,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X164"/>
+  <dimension ref="A1:Y164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V80" sqref="V80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2055,7 +2239,7 @@
     <col min="19" max="19" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2119,8 +2303,11 @@
       <c r="U1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2181,11 +2368,11 @@
       <c r="T2">
         <v>-2.271998</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2246,11 +2433,11 @@
       <c r="T3">
         <v>-1.7989189999999999</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2311,11 +2498,11 @@
       <c r="T4">
         <v>-1.3955090000000001</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2376,11 +2563,11 @@
       <c r="T5">
         <v>-1.12195</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2442,7 +2629,7 @@
         <v>-1.1126799999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2504,7 +2691,7 @@
         <v>-1.036095</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2565,14 +2752,14 @@
       <c r="T8">
         <v>-1.0079009999999999</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>246</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2633,18 +2820,18 @@
       <c r="T9">
         <v>-0.97209400000000001</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>238</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f>MEDIAN(T62:T65,T80,T83:T85)</f>
         <v>-1.5884845000000001</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>-0.98531449999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2705,18 +2892,18 @@
       <c r="T10">
         <v>-0.89863099999999996</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>239</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <f>STDEV(T62:T65,T80,T83:T85)</f>
         <v>0.23471135467085555</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>9.8001259436422558E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2777,18 +2964,18 @@
       <c r="T11">
         <v>-0.79697399999999996</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>244</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f>MIN(T62:T65,T80,T83:T85)</f>
         <v>-2.2282899999999999</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>-1.1408739999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2849,18 +3036,18 @@
       <c r="T12">
         <v>-0.793852</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>245</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f>MAX(T62:T65,T80,T83:T85)</f>
         <v>-1.5236069999999999</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>-0.87365499999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2922,7 +3109,7 @@
         <v>-0.75199300000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2983,15 +3170,15 @@
       <c r="T14">
         <v>-0.69716599999999995</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>240</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <f>MEDIAN(T75:T76,T78:T79,T93:T96)</f>
         <v>-0.98531449999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3052,15 +3239,15 @@
       <c r="T15">
         <v>-0.64887099999999998</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>241</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <f>STDEV(T75:T76,T78:T79,T93:T96)</f>
         <v>9.8001259436422558E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3121,15 +3308,15 @@
       <c r="T16">
         <v>-0.406532</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>242</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <f>MIN(T75:T76,T78:T79,T93:T96)</f>
         <v>-1.1408739999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3190,15 +3377,15 @@
       <c r="T17">
         <v>-1.8908259999999999</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>243</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <f>MAX(T75:T76,T78:T79,T93:T96)</f>
         <v>-0.87365499999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3260,7 +3447,7 @@
         <v>-1.579995</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3322,7 +3509,7 @@
         <v>-1.462728</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3384,7 +3571,7 @@
         <v>-1.3612629999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3446,7 +3633,7 @@
         <v>-1.3347260000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3508,7 +3695,7 @@
         <v>-1.31609</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3570,7 +3757,7 @@
         <v>-1.223703</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -3632,7 +3819,7 @@
         <v>-1.1940440000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -3694,7 +3881,7 @@
         <v>-1.181748</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3756,7 +3943,7 @@
         <v>-1.011023</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -3818,7 +4005,7 @@
         <v>-0.91268000000000005</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3880,7 +4067,7 @@
         <v>-0.89229099999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3942,7 +4129,7 @@
         <v>-0.83131600000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -4004,7 +4191,7 @@
         <v>-0.79853499999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -4066,7 +4253,7 @@
         <v>-0.60009599999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3</v>
       </c>
@@ -6118,7 +6305,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16">
         <v>1</v>
       </c>
@@ -6183,7 +6370,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>2</v>
       </c>
@@ -6247,8 +6434,11 @@
       <c r="U66" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V66" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>3</v>
       </c>
@@ -6312,8 +6502,11 @@
       <c r="U67" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V67" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>4</v>
       </c>
@@ -6375,7 +6568,7 @@
         <v>-1.353362</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>4</v>
       </c>
@@ -6439,8 +6632,11 @@
       <c r="U69" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V69" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="10">
         <v>2</v>
       </c>
@@ -6505,7 +6701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>4</v>
       </c>
@@ -6567,7 +6763,7 @@
         <v>-1.2643850000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>3</v>
       </c>
@@ -6631,8 +6827,11 @@
       <c r="U72" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V72" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
         <v>2</v>
       </c>
@@ -6697,7 +6896,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>4</v>
       </c>
@@ -6762,7 +6961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="13">
         <v>3</v>
       </c>
@@ -6827,7 +7026,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="13">
         <v>4</v>
       </c>
@@ -6888,8 +7087,11 @@
       <c r="T76" s="13">
         <v>-0.97824199999999994</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V76" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
         <v>1</v>
       </c>
@@ -6951,7 +7153,7 @@
         <v>-0.94423599999999996</v>
       </c>
     </row>
-    <row r="78" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="13">
         <v>1</v>
       </c>
@@ -7012,8 +7214,11 @@
       <c r="T78" s="13">
         <v>-0.94418800000000003</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V78" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="13">
         <v>2</v>
       </c>
@@ -7074,8 +7279,11 @@
       <c r="T79" s="13">
         <v>-0.87365499999999996</v>
       </c>
-    </row>
-    <row r="80" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V79" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16">
         <v>3</v>
       </c>
@@ -7137,7 +7345,7 @@
         <v>-1.7595099999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="19">
         <v>1</v>
       </c>
@@ -7198,8 +7406,11 @@
       <c r="T81" s="19">
         <v>-1.706628</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V81" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="19">
         <v>2</v>
       </c>
@@ -7260,8 +7471,11 @@
       <c r="T82" s="19">
         <v>-1.6676029999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V82" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16">
         <v>3</v>
       </c>
@@ -7323,7 +7537,7 @@
         <v>-1.608093</v>
       </c>
     </row>
-    <row r="84" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16">
         <v>4</v>
       </c>
@@ -7388,7 +7602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16">
         <v>2</v>
       </c>
@@ -7453,7 +7667,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>1</v>
       </c>
@@ -7517,8 +7731,11 @@
       <c r="U86" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V86" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>4</v>
       </c>
@@ -7580,7 +7797,7 @@
         <v>-1.476777</v>
       </c>
     </row>
-    <row r="88" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="10">
         <v>4</v>
       </c>
@@ -7645,7 +7862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="10">
         <v>2</v>
       </c>
@@ -7710,7 +7927,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>4</v>
       </c>
@@ -7772,7 +7989,7 @@
         <v>-1.2409699999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>3</v>
       </c>
@@ -7836,8 +8053,11 @@
       <c r="U91" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="92" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V91" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="10">
         <v>1</v>
       </c>
@@ -7902,7 +8122,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13">
         <v>2</v>
       </c>
@@ -7967,7 +8187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13">
         <v>4</v>
       </c>
@@ -8029,7 +8249,7 @@
         <v>-1.098535</v>
       </c>
     </row>
-    <row r="95" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13">
         <v>1</v>
       </c>
@@ -8090,8 +8310,11 @@
       <c r="T95" s="13">
         <v>-0.99238700000000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V95" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13">
         <v>3</v>
       </c>
@@ -8151,6 +8374,9 @@
       </c>
       <c r="T96" s="13">
         <v>-0.94068200000000002</v>
+      </c>
+      <c r="V96" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.2">
@@ -10137,7 +10363,7 @@
         <v>-0.78009099999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1</v>
       </c>
@@ -10199,7 +10425,7 @@
         <v>-0.74565300000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2</v>
       </c>
@@ -10261,7 +10487,7 @@
         <v>-0.71306400000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="16">
         <v>2</v>
       </c>
@@ -10323,7 +10549,7 @@
         <v>-1.5613589999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="16">
         <v>4</v>
       </c>
@@ -10385,7 +10611,7 @@
         <v>-1.473751</v>
       </c>
     </row>
-    <row r="133" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="16">
         <v>3</v>
       </c>
@@ -10447,7 +10673,7 @@
         <v>-1.3922909999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="16">
         <v>4</v>
       </c>
@@ -10509,7 +10735,7 @@
         <v>-1.2735590000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>3</v>
       </c>
@@ -10570,8 +10796,11 @@
       <c r="T135">
         <v>-1.119116</v>
       </c>
-    </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V135" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2</v>
       </c>
@@ -10632,8 +10861,11 @@
       <c r="T136">
         <v>-1.0425310000000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V136" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>4</v>
       </c>
@@ -10695,7 +10927,7 @@
         <v>-0.92516799999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2</v>
       </c>
@@ -10757,7 +10989,7 @@
         <v>-0.88146000000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>4</v>
       </c>
@@ -10819,7 +11051,7 @@
         <v>-0.80175300000000005</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2</v>
       </c>
@@ -10881,7 +11113,7 @@
         <v>-0.78155600000000003</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>4</v>
       </c>
@@ -10942,8 +11174,11 @@
       <c r="T141">
         <v>-0.67989900000000003</v>
       </c>
-    </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="V141" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="142" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>1</v>
       </c>
@@ -11004,8 +11239,11 @@
       <c r="T142">
         <v>-0.64390000000000003</v>
       </c>
-    </row>
-    <row r="143" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V142" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="143" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="13">
         <v>4</v>
       </c>
@@ -11067,7 +11305,7 @@
         <v>-0.64077799999999996</v>
       </c>
     </row>
-    <row r="144" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:22" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="13">
         <v>1</v>
       </c>
@@ -12386,7 +12624,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -12428,19 +12666,25 @@
       <c r="H1" s="25" t="s">
         <v>248</v>
       </c>
+      <c r="I1" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>298</v>
+      </c>
       <c r="L1" s="23" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="27">
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>23</v>
@@ -12449,30 +12693,36 @@
         <v>24</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G2" s="26">
-        <v>-0.99238700000000002</v>
+        <v>-0.94418800000000003</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>249</v>
       </c>
+      <c r="I2" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>294</v>
+      </c>
       <c r="L2" s="24">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>24</v>
@@ -12481,10 +12731,16 @@
         <v>33</v>
       </c>
       <c r="G3" s="26">
-        <v>-1.262632</v>
+        <v>-1.5891690000000001</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>250</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>293</v>
       </c>
       <c r="L3" s="24">
         <v>15</v>
@@ -12495,10 +12751,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>218</v>
+        <v>56</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>40</v>
@@ -12510,10 +12766,16 @@
         <v>33</v>
       </c>
       <c r="G4" s="26">
-        <v>-0.31296800000000002</v>
+        <v>-1.475312</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>296</v>
       </c>
       <c r="L4" s="24">
         <v>1</v>
@@ -12521,28 +12783,34 @@
     </row>
     <row r="5" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>51</v>
+        <v>182</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E5" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G5" s="26">
-        <v>-1.547118</v>
+        <v>-0.57706500000000005</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>292</v>
       </c>
       <c r="L5" s="24">
         <v>28</v>
@@ -12550,16 +12818,16 @@
     </row>
     <row r="6" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
+        <v>1</v>
+      </c>
+      <c r="B6" s="27">
         <v>3</v>
       </c>
-      <c r="B6" s="27">
-        <v>1</v>
-      </c>
       <c r="C6" s="25" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E6" s="25" t="s">
         <v>24</v>
@@ -12568,10 +12836,16 @@
         <v>25</v>
       </c>
       <c r="G6" s="26">
-        <v>-0.52048499999999998</v>
+        <v>-1.5878000000000001</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>297</v>
       </c>
       <c r="L6" s="24">
         <v>18</v>
@@ -12582,13 +12856,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>24</v>
@@ -12597,10 +12871,16 @@
         <v>25</v>
       </c>
       <c r="G7" s="26">
-        <v>-0.94418800000000003</v>
+        <v>-1.5613589999999999</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="L7" s="24">
         <v>7</v>
@@ -12608,13 +12888,13 @@
     </row>
     <row r="8" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>23</v>
@@ -12626,10 +12906,16 @@
         <v>25</v>
       </c>
       <c r="G8" s="26">
-        <v>-2.2282899999999999</v>
+        <v>-0.87365499999999996</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="L8" s="24">
         <v>27</v>
@@ -12637,28 +12923,34 @@
     </row>
     <row r="9" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="27">
         <v>1</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>37</v>
+        <v>218</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G9" s="26">
-        <v>-1.5582370000000001</v>
+        <v>-0.31296800000000002</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="L9" s="24">
         <v>14</v>
@@ -12666,28 +12958,34 @@
     </row>
     <row r="10" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>203</v>
+        <v>57</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G10" s="26">
-        <v>-0.56438500000000003</v>
+        <v>-1.5236069999999999</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>294</v>
       </c>
       <c r="L10" s="24">
         <v>17</v>
@@ -12698,13 +12996,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>24</v>
@@ -12713,24 +13011,30 @@
         <v>33</v>
       </c>
       <c r="G11" s="26">
-        <v>-1.5236069999999999</v>
+        <v>-1.262632</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>250</v>
       </c>
+      <c r="I11" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>293</v>
+      </c>
       <c r="L11" s="24">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="27">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>40</v>
@@ -12739,13 +13043,19 @@
         <v>24</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G12" s="26">
-        <v>-0.85667599999999999</v>
+        <v>-0.64077799999999996</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>249</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>296</v>
       </c>
       <c r="L12" s="24">
         <v>24</v>
@@ -12756,10 +13066,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>207</v>
+        <v>93</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>40</v>
@@ -12768,13 +13078,19 @@
         <v>24</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G13" s="26">
-        <v>-0.51599399999999995</v>
+        <v>-1.3922909999999999</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>292</v>
       </c>
       <c r="L13" s="24">
         <v>10</v>
@@ -12782,13 +13098,13 @@
     </row>
     <row r="14" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="27">
         <v>2</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>40</v>
@@ -12800,24 +13116,30 @@
         <v>33</v>
       </c>
       <c r="G14" s="26">
-        <v>-0.57706500000000005</v>
+        <v>-0.51599399999999995</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>249</v>
       </c>
+      <c r="I14" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>297</v>
+      </c>
       <c r="L14" s="24">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>23</v>
@@ -12829,24 +13151,30 @@
         <v>33</v>
       </c>
       <c r="G15" s="26">
-        <v>-1.1408739999999999</v>
+        <v>-0.99238700000000002</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>249</v>
       </c>
+      <c r="I15" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>291</v>
+      </c>
       <c r="L15" s="24">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
+        <v>2</v>
+      </c>
+      <c r="B16" s="27">
         <v>1</v>
       </c>
-      <c r="B16" s="27">
-        <v>2</v>
-      </c>
       <c r="C16" s="25" t="s">
-        <v>178</v>
+        <v>37</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>23</v>
@@ -12858,10 +13186,16 @@
         <v>25</v>
       </c>
       <c r="G16" s="26">
-        <v>-0.87365499999999996</v>
+        <v>-1.5582370000000001</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="L16" s="24">
         <v>5</v>
@@ -12869,28 +13203,34 @@
     </row>
     <row r="17" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>38</v>
+        <v>196</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G17" s="26">
-        <v>-1.5613589999999999</v>
+        <v>-0.94068200000000002</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="L17" s="24">
         <v>3</v>
@@ -12898,13 +13238,13 @@
     </row>
     <row r="18" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
+        <v>3</v>
+      </c>
+      <c r="B18" s="27">
         <v>4</v>
       </c>
-      <c r="B18" s="27">
-        <v>3</v>
-      </c>
       <c r="C18" s="25" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>23</v>
@@ -12913,13 +13253,19 @@
         <v>24</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G18" s="26">
-        <v>-1.7595099999999999</v>
+        <v>-0.97824199999999994</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>294</v>
       </c>
       <c r="L18" s="24">
         <v>30</v>
@@ -12927,42 +13273,48 @@
     </row>
     <row r="19" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G19" s="26">
-        <v>-0.94068200000000002</v>
+        <v>-0.52048499999999998</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>249</v>
       </c>
+      <c r="I19" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>293</v>
+      </c>
       <c r="L19" s="24">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
+        <v>3</v>
+      </c>
+      <c r="B20" s="27">
         <v>4</v>
       </c>
-      <c r="B20" s="27">
-        <v>3</v>
-      </c>
       <c r="C20" s="25" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>40</v>
@@ -12971,13 +13323,19 @@
         <v>24</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G20" s="26">
-        <v>-1.731508</v>
+        <v>-1.473751</v>
       </c>
       <c r="H20" s="25" t="s">
         <v>250</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>296</v>
       </c>
       <c r="L20" s="24">
         <v>32</v>
@@ -12988,13 +13346,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>24</v>
@@ -13003,10 +13361,16 @@
         <v>33</v>
       </c>
       <c r="G21" s="26">
-        <v>-1.608093</v>
+        <v>-0.85667599999999999</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>292</v>
       </c>
       <c r="L21" s="24">
         <v>23</v>
@@ -13014,16 +13378,16 @@
     </row>
     <row r="22" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22" s="27">
         <v>3</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>50</v>
+        <v>231</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>24</v>
@@ -13032,10 +13396,16 @@
         <v>25</v>
       </c>
       <c r="G22" s="26">
-        <v>-1.5878000000000001</v>
+        <v>-0.29394799999999999</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="J22" s="34" t="s">
+        <v>297</v>
       </c>
       <c r="L22" s="24">
         <v>8</v>
@@ -13043,13 +13413,13 @@
     </row>
     <row r="23" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>93</v>
+        <v>203</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>40</v>
@@ -13061,10 +13431,16 @@
         <v>25</v>
       </c>
       <c r="G23" s="26">
-        <v>-1.3922909999999999</v>
+        <v>-0.56438500000000003</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="J23" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="L23" s="24">
         <v>13</v>
@@ -13078,22 +13454,28 @@
         <v>3</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>231</v>
+        <v>47</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G24" s="26">
-        <v>-0.29394799999999999</v>
+        <v>-1.608093</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="L24" s="24">
         <v>21</v>
@@ -13101,13 +13483,13 @@
     </row>
     <row r="25" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>23</v>
@@ -13116,13 +13498,19 @@
         <v>24</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G25" s="26">
-        <v>-1.1250720000000001</v>
+        <v>-1.1408739999999999</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>249</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="J25" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="L25" s="24">
         <v>25</v>
@@ -13133,13 +13521,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>158</v>
+        <v>44</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>24</v>
@@ -13148,10 +13536,16 @@
         <v>33</v>
       </c>
       <c r="G26" s="26">
-        <v>-1.098535</v>
+        <v>-1.731508</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>294</v>
       </c>
       <c r="L26" s="24">
         <v>29</v>
@@ -13159,16 +13553,16 @@
     </row>
     <row r="27" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B27" s="27">
         <v>4</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>24</v>
@@ -13177,10 +13571,16 @@
         <v>33</v>
       </c>
       <c r="G27" s="26">
-        <v>-1.475312</v>
+        <v>-1.098535</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>293</v>
       </c>
       <c r="L27" s="24">
         <v>4</v>
@@ -13191,42 +13591,48 @@
         <v>4</v>
       </c>
       <c r="B28" s="27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G28" s="26">
-        <v>-1.520389</v>
+        <v>-2.2282899999999999</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>250</v>
       </c>
+      <c r="I28" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>296</v>
+      </c>
       <c r="L28" s="24">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B29" s="27">
         <v>4</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E29" s="25" t="s">
         <v>24</v>
@@ -13235,10 +13641,16 @@
         <v>33</v>
       </c>
       <c r="G29" s="26">
-        <v>-1.5891690000000001</v>
+        <v>-1.520389</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>250</v>
+      </c>
+      <c r="I29" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>292</v>
       </c>
       <c r="L29" s="24">
         <v>6</v>
@@ -13249,13 +13661,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>24</v>
@@ -13264,27 +13676,33 @@
         <v>25</v>
       </c>
       <c r="G30" s="26">
-        <v>-1.2735590000000001</v>
+        <v>-1.547118</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>250</v>
       </c>
+      <c r="I30" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="J30" s="34" t="s">
+        <v>297</v>
+      </c>
       <c r="L30" s="24">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" s="27">
         <v>4</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>190</v>
+        <v>122</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>24</v>
@@ -13293,10 +13711,16 @@
         <v>25</v>
       </c>
       <c r="G31" s="26">
-        <v>-0.97824199999999994</v>
+        <v>-1.2735590000000001</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="J31" s="34" t="s">
+        <v>291</v>
       </c>
       <c r="L31" s="24">
         <v>20</v>
@@ -13304,28 +13728,34 @@
     </row>
     <row r="32" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B32" s="27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>223</v>
+        <v>46</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E32" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G32" s="26">
-        <v>-0.64077799999999996</v>
+        <v>-1.7595099999999999</v>
       </c>
       <c r="H32" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
+      </c>
+      <c r="I32" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>295</v>
       </c>
       <c r="L32" s="24">
         <v>9</v>
@@ -13333,16 +13763,16 @@
     </row>
     <row r="33" spans="1:12" ht="20" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
+        <v>4</v>
+      </c>
+      <c r="B33" s="27">
         <v>3</v>
       </c>
-      <c r="B33" s="27">
-        <v>4</v>
-      </c>
       <c r="C33" s="25" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="E33" s="25" t="s">
         <v>24</v>
@@ -13351,10 +13781,16 @@
         <v>25</v>
       </c>
       <c r="G33" s="26">
-        <v>-1.473751</v>
+        <v>-1.1250720000000001</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="J33" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="L33" s="24">
         <v>22</v>

</xml_diff>